<commit_message>
Update on Report and improvements files
</commit_message>
<xml_diff>
--- a/Issues-and-Improvements-of-MaintainX.xlsx
+++ b/Issues-and-Improvements-of-MaintainX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27809"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5953502-5ED4-4D15-9E92-AEC6AFCC74FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1B36747-0AFB-4E5A-B329-F9E3314A4AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>TC#</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Search results should accurately display work orders matching the search criteria.</t>
+  </si>
+  <si>
+    <t>Pagination mechanism is missing in the View Work-Orders list</t>
+  </si>
+  <si>
+    <t>Pagination controls should be present at the bottom of the work-orders list. If pagination is missing, all work orders are displayed on a single page, leading to potential performance issues and poor user experience.</t>
   </si>
 </sst>
 </file>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -685,14 +691,25 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>